<commit_message>
Lan thay doi on thu 2
</commit_message>
<xml_diff>
--- a/Child.xlsx
+++ b/Child.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1515" uniqueCount="1012">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1525" uniqueCount="1012">
   <si>
     <t>No</t>
   </si>
@@ -3941,13 +3941,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="A7" sqref="$A7:$XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.06666666666667" defaultRowHeight="14.25" outlineLevelRow="5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.06666666666667" defaultRowHeight="14.25" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="3" width="9"/>
   </cols>
@@ -4016,6 +4016,61 @@
       </c>
       <c r="C6" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>1956</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>1957</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>1958</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>1959</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>1960</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -4030,7 +4085,7 @@
   <dimension ref="A1:C751"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="$A2:$XFD6"/>
+      <selection activeCell="A7" sqref="$A7:$XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="2"/>

</xml_diff>

<commit_message>
Sua loi khi import File Excel bam cancle hien lai cua so import file
</commit_message>
<xml_diff>
--- a/Child.xlsx
+++ b/Child.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23145" windowHeight="9600"/>
+    <workbookView windowWidth="23145" windowHeight="8880"/>
   </bookViews>
   <sheets>
     <sheet name="Child" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1570" uniqueCount="1012">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="1012">
   <si>
     <t>No</t>
   </si>
@@ -3941,10 +3941,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="$A12:$XFD34"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.06666666666667" defaultRowHeight="14.25" outlineLevelCol="2"/>
@@ -4115,215 +4115,6 @@
       </c>
       <c r="C15" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16">
-        <v>1965</v>
-      </c>
-      <c r="B16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17">
-        <v>1966</v>
-      </c>
-      <c r="B17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18">
-        <v>1967</v>
-      </c>
-      <c r="B18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19">
-        <v>1968</v>
-      </c>
-      <c r="B19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20">
-        <v>1969</v>
-      </c>
-      <c r="B20" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21">
-        <v>1970</v>
-      </c>
-      <c r="B21" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22">
-        <v>1971</v>
-      </c>
-      <c r="B22" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23">
-        <v>1972</v>
-      </c>
-      <c r="B23" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24">
-        <v>1973</v>
-      </c>
-      <c r="B24" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25">
-        <v>1974</v>
-      </c>
-      <c r="B25" t="s">
-        <v>47</v>
-      </c>
-      <c r="C25" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26">
-        <v>1975</v>
-      </c>
-      <c r="B26" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27">
-        <v>1976</v>
-      </c>
-      <c r="B27" t="s">
-        <v>51</v>
-      </c>
-      <c r="C27" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28">
-        <v>1977</v>
-      </c>
-      <c r="B28" t="s">
-        <v>53</v>
-      </c>
-      <c r="C28">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29">
-        <v>1978</v>
-      </c>
-      <c r="B29" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30">
-        <v>1979</v>
-      </c>
-      <c r="B30" t="s">
-        <v>56</v>
-      </c>
-      <c r="C30" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31">
-        <v>1980</v>
-      </c>
-      <c r="B31" t="s">
-        <v>58</v>
-      </c>
-      <c r="C31" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32">
-        <v>1981</v>
-      </c>
-      <c r="B32" t="s">
-        <v>60</v>
-      </c>
-      <c r="C32" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33">
-        <v>1982</v>
-      </c>
-      <c r="B33" t="s">
-        <v>62</v>
-      </c>
-      <c r="C33" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34">
-        <v>1983</v>
-      </c>
-      <c r="B34" t="s">
-        <v>64</v>
-      </c>
-      <c r="C34" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dieu chinh lai ket qua luon hien thi dong moi nhat tai dong dau tien
</commit_message>
<xml_diff>
--- a/Child.xlsx
+++ b/Child.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23145" windowHeight="8880"/>
+    <workbookView windowWidth="23145" windowHeight="9600"/>
   </bookViews>
   <sheets>
     <sheet name="Child" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="1012">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1568" uniqueCount="1012">
   <si>
     <t>No</t>
   </si>
@@ -96,139 +96,139 @@
     <t>Opposite Acme Gulmohar Heights, Near Gopal Sweets, Chandigarh Kharar Highway - 140301</t>
   </si>
   <si>
+    <t>Capital O 92615 Villa Utama D'alas Purwo</t>
+  </si>
+  <si>
+    <t>01, Banyuwangi, Jawa Timur</t>
+  </si>
+  <si>
+    <t>EagleRedCasino</t>
+  </si>
+  <si>
+    <t>Near Thangalpara Kolahalamedu - Elamkadu Road</t>
+  </si>
+  <si>
+    <t>Hotel SD Grand Palace</t>
+  </si>
+  <si>
+    <t>Mant Raya Road , Near Sri Radha Rani Temple And Bansiwat Temple</t>
+  </si>
+  <si>
+    <t>Sukha Retreats</t>
+  </si>
+  <si>
+    <t>P O, Peringazha, Hmt Colony, North Kalamassery, Kalamassery, Kochi, Kerala 683503</t>
+  </si>
+  <si>
+    <t>HOTEL TASIK UTAMA , AYER KEROH , MELAKA</t>
+  </si>
+  <si>
+    <t>97   99 Jalan Tu 3</t>
+  </si>
+  <si>
+    <t>Namasthe Ayurveda and Yoga Retreat</t>
+  </si>
+  <si>
+    <t>Karakkattukunnu Chira -Mekkad P.O, Mekkad Namasthe Ayurveda And Yoga Retreat Namasthe Ayurveda And Yoga Retreat</t>
+  </si>
+  <si>
+    <t>Beijing Hai'an Hotel (Yuanmingyuan Sports University Shangdi Branch)</t>
+  </si>
+  <si>
+    <t>No.38 Xinxi Road, Haidian District, Beijing, China</t>
+  </si>
+  <si>
+    <t>Treebo Trip Sun Square</t>
+  </si>
+  <si>
+    <t>D. No 26/6/4, Papaiah Street</t>
+  </si>
+  <si>
+    <t>Vienna Hotel (Guangzhou Huadu Sunac Resort Snow Miracle)</t>
+  </si>
+  <si>
+    <t>No.160 Shuguang Road</t>
+  </si>
+  <si>
+    <t>Qiancheng Hotel (Kunming Xishan Wanda Plaza)</t>
+  </si>
+  <si>
+    <t>5F, Building22-5, Phase 4, Greenland Dacheng Tiandi, Qianwei West Road</t>
+  </si>
+  <si>
+    <t>Vienna Hotel (Beijing Wanda West, Bajiao Amusement Park Metro Station)</t>
+  </si>
+  <si>
+    <t>No.23 Shijingshan Road</t>
+  </si>
+  <si>
+    <t>New Century Manju Hotel</t>
+  </si>
+  <si>
+    <t>29 North Yanhe Road (Yanhe Bei Lu)</t>
+  </si>
+  <si>
+    <t>Aour Hotel, Dazhi Road, Suning square, Huaiï¼‡an city</t>
+  </si>
+  <si>
+    <t>No. 10, Dazhi West Road</t>
+  </si>
+  <si>
+    <t>Hanting Hotel (Shanghai Wujiaochang Huangxing Road)</t>
+  </si>
+  <si>
+    <t>3F, Wujiaochang Technology Building, No.1675 Huangxing Road</t>
+  </si>
+  <si>
+    <t>Comfort Inn Xinzheng (Zhengzhou Xinzheng International Airport)</t>
+  </si>
+  <si>
+    <t>Near No.203 Provincial Road</t>
+  </si>
+  <si>
+    <t>Haiyou Hotel (Hangzhou West Lake Avenue)</t>
+  </si>
+  <si>
+    <t>Dream Love Hotel (Xinzheng International Airport)</t>
+  </si>
+  <si>
+    <t>No. 35-1, Yungang Road, Aviation Port District</t>
+  </si>
+  <si>
+    <t>Motel 168 (Shanghai Wuning Road Metro Station Anyuan Road)</t>
+  </si>
+  <si>
+    <t>No.678 Anyuan Road</t>
+  </si>
+  <si>
+    <t>Aidu Hotel (Xinzheng International Airport)</t>
+  </si>
+  <si>
+    <t>No. 29-3, Yungang Road, Aviation Port District</t>
+  </si>
+  <si>
+    <t>Atour Hotel Renmin University Beijing Zhongguancun</t>
+  </si>
+  <si>
+    <t>Building 67, No. 3, Tonghui Temple, Haidian, Beijing, Beijing, Haidian District, China</t>
+  </si>
+  <si>
+    <t>Shangkeyou Express Hotel (Jiaokou Chengxi Street Branch)</t>
+  </si>
+  <si>
+    <t>Houshui Bridge Head</t>
+  </si>
+  <si>
+    <t>Hotel Tasik Utama</t>
+  </si>
+  <si>
+    <t>Jalan Tu 3, Taman Tasik Utama, 97 &amp; 99</t>
+  </si>
+  <si>
     <t>Taru Villas Maia - Habarana</t>
   </si>
   <si>
     <t>Habarana Road</t>
-  </si>
-  <si>
-    <t>Capital O 92615 Villa Utama D'alas Purwo</t>
-  </si>
-  <si>
-    <t>01, Banyuwangi, Jawa Timur</t>
-  </si>
-  <si>
-    <t>EagleRedCasino</t>
-  </si>
-  <si>
-    <t>Near Thangalpara Kolahalamedu - Elamkadu Road</t>
-  </si>
-  <si>
-    <t>Hotel SD Grand Palace</t>
-  </si>
-  <si>
-    <t>Mant Raya Road , Near Sri Radha Rani Temple And Bansiwat Temple</t>
-  </si>
-  <si>
-    <t>Sukha Retreats</t>
-  </si>
-  <si>
-    <t>P O, Peringazha, Hmt Colony, North Kalamassery, Kalamassery, Kochi, Kerala 683503</t>
-  </si>
-  <si>
-    <t>HOTEL TASIK UTAMA , AYER KEROH , MELAKA</t>
-  </si>
-  <si>
-    <t>97   99 Jalan Tu 3</t>
-  </si>
-  <si>
-    <t>Namasthe Ayurveda and Yoga Retreat</t>
-  </si>
-  <si>
-    <t>Karakkattukunnu Chira -Mekkad P.O, Mekkad Namasthe Ayurveda And Yoga Retreat Namasthe Ayurveda And Yoga Retreat</t>
-  </si>
-  <si>
-    <t>Beijing Hai'an Hotel (Yuanmingyuan Sports University Shangdi Branch)</t>
-  </si>
-  <si>
-    <t>No.38 Xinxi Road, Haidian District, Beijing, China</t>
-  </si>
-  <si>
-    <t>Treebo Trip Sun Square</t>
-  </si>
-  <si>
-    <t>D. No 26/6/4, Papaiah Street</t>
-  </si>
-  <si>
-    <t>Vienna Hotel (Guangzhou Huadu Sunac Resort Snow Miracle)</t>
-  </si>
-  <si>
-    <t>No.160 Shuguang Road</t>
-  </si>
-  <si>
-    <t>Qiancheng Hotel (Kunming Xishan Wanda Plaza)</t>
-  </si>
-  <si>
-    <t>5F, Building22-5, Phase 4, Greenland Dacheng Tiandi, Qianwei West Road</t>
-  </si>
-  <si>
-    <t>Vienna Hotel (Beijing Wanda West, Bajiao Amusement Park Metro Station)</t>
-  </si>
-  <si>
-    <t>No.23 Shijingshan Road</t>
-  </si>
-  <si>
-    <t>New Century Manju Hotel</t>
-  </si>
-  <si>
-    <t>29 North Yanhe Road (Yanhe Bei Lu)</t>
-  </si>
-  <si>
-    <t>Aour Hotel, Dazhi Road, Suning square, Huaiï¼‡an city</t>
-  </si>
-  <si>
-    <t>No. 10, Dazhi West Road</t>
-  </si>
-  <si>
-    <t>Hanting Hotel (Shanghai Wujiaochang Huangxing Road)</t>
-  </si>
-  <si>
-    <t>3F, Wujiaochang Technology Building, No.1675 Huangxing Road</t>
-  </si>
-  <si>
-    <t>Comfort Inn Xinzheng (Zhengzhou Xinzheng International Airport)</t>
-  </si>
-  <si>
-    <t>Near No.203 Provincial Road</t>
-  </si>
-  <si>
-    <t>Haiyou Hotel (Hangzhou West Lake Avenue)</t>
-  </si>
-  <si>
-    <t>Dream Love Hotel (Xinzheng International Airport)</t>
-  </si>
-  <si>
-    <t>No. 35-1, Yungang Road, Aviation Port District</t>
-  </si>
-  <si>
-    <t>Motel 168 (Shanghai Wuning Road Metro Station Anyuan Road)</t>
-  </si>
-  <si>
-    <t>No.678 Anyuan Road</t>
-  </si>
-  <si>
-    <t>Aidu Hotel (Xinzheng International Airport)</t>
-  </si>
-  <si>
-    <t>No. 29-3, Yungang Road, Aviation Port District</t>
-  </si>
-  <si>
-    <t>Atour Hotel Renmin University Beijing Zhongguancun</t>
-  </si>
-  <si>
-    <t>Building 67, No. 3, Tonghui Temple, Haidian, Beijing, Beijing, Haidian District, China</t>
-  </si>
-  <si>
-    <t>Shangkeyou Express Hotel (Jiaokou Chengxi Street Branch)</t>
-  </si>
-  <si>
-    <t>Houshui Bridge Head</t>
-  </si>
-  <si>
-    <t>Hotel Tasik Utama</t>
-  </si>
-  <si>
-    <t>Jalan Tu 3, Taman Tasik Utama, 97 &amp; 99</t>
   </si>
   <si>
     <t>Gurjeet Hotel by Naavagat</t>
@@ -3941,10 +3941,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.06666666666667" defaultRowHeight="14.25" outlineLevelCol="2"/>
@@ -4064,7 +4064,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
-        <v>1960</v>
+        <v>1961</v>
       </c>
       <c r="B11" t="s">
         <v>21</v>
@@ -4075,7 +4075,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <v>1961</v>
+        <v>1962</v>
       </c>
       <c r="B12" t="s">
         <v>23</v>
@@ -4086,7 +4086,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>1962</v>
+        <v>1963</v>
       </c>
       <c r="B13" t="s">
         <v>25</v>
@@ -4097,7 +4097,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>1963</v>
+        <v>1964</v>
       </c>
       <c r="B14" t="s">
         <v>27</v>
@@ -4108,13 +4108,211 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15">
-        <v>1964</v>
+        <v>1965</v>
       </c>
       <c r="B15" t="s">
         <v>29</v>
       </c>
       <c r="C15" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>1966</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>1967</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>1968</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>1969</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20">
+        <v>1970</v>
+      </c>
+      <c r="B20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>1971</v>
+      </c>
+      <c r="B21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22">
+        <v>1972</v>
+      </c>
+      <c r="B22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <v>1973</v>
+      </c>
+      <c r="B23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>1974</v>
+      </c>
+      <c r="B24" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25">
+        <v>1975</v>
+      </c>
+      <c r="B25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26">
+        <v>1976</v>
+      </c>
+      <c r="B26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27">
+        <v>1977</v>
+      </c>
+      <c r="B27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28">
+        <v>1978</v>
+      </c>
+      <c r="B28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29">
+        <v>1979</v>
+      </c>
+      <c r="B29" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30">
+        <v>1980</v>
+      </c>
+      <c r="B30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31">
+        <v>1981</v>
+      </c>
+      <c r="B31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32">
+        <v>1982</v>
+      </c>
+      <c r="B32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33">
+        <v>1983</v>
+      </c>
+      <c r="B33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -4249,10 +4447,10 @@
         <v>1960</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -4260,10 +4458,10 @@
         <v>1961</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -4271,10 +4469,10 @@
         <v>1962</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -4282,10 +4480,10 @@
         <v>1963</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -4293,10 +4491,10 @@
         <v>1964</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -4304,10 +4502,10 @@
         <v>1965</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -4315,10 +4513,10 @@
         <v>1966</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -4326,10 +4524,10 @@
         <v>1967</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -4337,10 +4535,10 @@
         <v>1968</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -4348,10 +4546,10 @@
         <v>1969</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -4359,10 +4557,10 @@
         <v>1970</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -4370,10 +4568,10 @@
         <v>1971</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -4381,10 +4579,10 @@
         <v>1972</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -4392,10 +4590,10 @@
         <v>1973</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -4403,10 +4601,10 @@
         <v>1974</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -4414,10 +4612,10 @@
         <v>1975</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C26" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -4425,10 +4623,10 @@
         <v>1976</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C27" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -4436,7 +4634,7 @@
         <v>1977</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C28">
         <v>486</v>
@@ -4447,10 +4645,10 @@
         <v>1978</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C29" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -4458,10 +4656,10 @@
         <v>1979</v>
       </c>
       <c r="B30" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -4469,10 +4667,10 @@
         <v>1980</v>
       </c>
       <c r="B31" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C31" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -4480,10 +4678,10 @@
         <v>1981</v>
       </c>
       <c r="B32" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C32" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -4491,10 +4689,10 @@
         <v>1982</v>
       </c>
       <c r="B33" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C33" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -4502,10 +4700,10 @@
         <v>1983</v>
       </c>
       <c r="B34" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C34" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -4601,10 +4799,10 @@
         <v>1992</v>
       </c>
       <c r="B43" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C43" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -4612,10 +4810,10 @@
         <v>1993</v>
       </c>
       <c r="B44" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C44" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -4645,10 +4843,10 @@
         <v>1996</v>
       </c>
       <c r="B47" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C47" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -4656,10 +4854,10 @@
         <v>1997</v>
       </c>
       <c r="B48" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C48" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -4667,10 +4865,10 @@
         <v>1998</v>
       </c>
       <c r="B49" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C49" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -4934,7 +5132,7 @@
         <v>118</v>
       </c>
       <c r="C73" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -5019,10 +5217,10 @@
         <v>2030</v>
       </c>
       <c r="B81" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C81" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="82" spans="1:3">

</xml_diff>